<commit_message>
Data Pooling 2.0 (procrastination)
</commit_message>
<xml_diff>
--- a/rubberstopper.xlsx
+++ b/rubberstopper.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9b9e08a6e1c3ade1/Chemistry Data Pooling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguye\OneDrive\Chemistry Data Pooling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45D80C4C-A904-40B3-8BBC-AA28A27C1946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78CB5200-0120-4D13-921D-62478344A2C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
   <si>
     <t xml:space="preserve">Group Name </t>
   </si>
@@ -56,9 +56,6 @@
     <t>Relative Uncertainty (%)</t>
   </si>
   <si>
-    <t>Winnie &amp; Lillian</t>
-  </si>
-  <si>
     <t>13 ± 4 cm^3</t>
   </si>
   <si>
@@ -74,9 +71,6 @@
     <t>31 %</t>
   </si>
   <si>
-    <t>Liad &amp; Eric</t>
-  </si>
-  <si>
     <t>25±1 cm^3</t>
   </si>
   <si>
@@ -89,9 +83,6 @@
     <t>0.4 kg/m^3</t>
   </si>
   <si>
-    <t>Lucas and Marcus</t>
-  </si>
-  <si>
     <t>13±2cm³</t>
   </si>
   <si>
@@ -104,9 +95,6 @@
     <t>82.7kg/m³</t>
   </si>
   <si>
-    <t>Angus and Haidee</t>
-  </si>
-  <si>
     <t>14 ± 10 cm³</t>
   </si>
   <si>
@@ -119,9 +107,6 @@
     <t>± 1.4×10³ kg/m³</t>
   </si>
   <si>
-    <t xml:space="preserve">Jolie and Jessica </t>
-  </si>
-  <si>
     <t>11.8±10</t>
   </si>
   <si>
@@ -131,9 +116,6 @@
     <t>1.29±0.8</t>
   </si>
   <si>
-    <t>Megan and angelinaaa</t>
-  </si>
-  <si>
     <t>12.4±5.0</t>
   </si>
   <si>
@@ -143,9 +125,6 @@
     <t>1.71 x 10^3</t>
   </si>
   <si>
-    <t>Annie and Gwyn</t>
-  </si>
-  <si>
     <t>13 ± 5</t>
   </si>
   <si>
@@ -155,9 +134,6 @@
     <t>1.6 x 10^3 kg/m</t>
   </si>
   <si>
-    <t xml:space="preserve">Cherrain and Ricky </t>
-  </si>
-  <si>
     <t xml:space="preserve">15 ± 2 cm³ </t>
   </si>
   <si>
@@ -170,9 +146,6 @@
     <t xml:space="preserve">1 x 10² kg/m³ </t>
   </si>
   <si>
-    <t>Matthew and Alex</t>
-  </si>
-  <si>
     <t>15+-2</t>
   </si>
   <si>
@@ -182,9 +155,6 @@
     <t>1.5x10 ^3 kg/m^3</t>
   </si>
   <si>
-    <t>Amy and May</t>
-  </si>
-  <si>
     <t>11±4 cm^3</t>
   </si>
   <si>
@@ -197,9 +167,6 @@
     <t>5x10^2 kg/m^3</t>
   </si>
   <si>
-    <t>Wilson and Edward</t>
-  </si>
-  <si>
     <t>17+-4</t>
   </si>
   <si>
@@ -209,9 +176,6 @@
     <t>(1.6+-0.4)E3</t>
   </si>
   <si>
-    <t>Kevin and Darren</t>
-  </si>
-  <si>
     <t>12+-4cm^3</t>
   </si>
   <si>
@@ -224,9 +188,6 @@
     <t>sixhundreds</t>
   </si>
   <si>
-    <t>Zihan and Khoa</t>
-  </si>
-  <si>
     <t>13 ± 3 mL</t>
   </si>
   <si>
@@ -239,9 +200,6 @@
     <t>± 0.4</t>
   </si>
   <si>
-    <t>Mohammad &amp; Ryan</t>
-  </si>
-  <si>
     <t>16 ± 10 cm³</t>
   </si>
   <si>
@@ -249,6 +207,45 @@
   </si>
   <si>
     <t>1.3*10^3 kg/m^3</t>
+  </si>
+  <si>
+    <t>WL</t>
+  </si>
+  <si>
+    <t>LE</t>
+  </si>
+  <si>
+    <t>LM</t>
+  </si>
+  <si>
+    <t>AH</t>
+  </si>
+  <si>
+    <t>JJ</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>AG</t>
+  </si>
+  <si>
+    <t>CR</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>WE</t>
+  </si>
+  <si>
+    <t>KD</t>
+  </si>
+  <si>
+    <t>ZK</t>
+  </si>
+  <si>
+    <t>MR</t>
   </si>
 </sst>
 </file>
@@ -269,14 +266,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
-      <color rgb="FFFF00FF"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -285,12 +281,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00FFFF"/>
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor rgb="FF00FFFF"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -300,181 +302,81 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF284E3F"/>
+        <color indexed="64"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
-        <color rgb="FF356854"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF284E3F"/>
+        <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="thin">
-        <color rgb="FF284E3F"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF356854"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF356854"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF284E3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
-        <color rgb="FF284E3F"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF356854"/>
-      </left>
+      <left/>
       <right style="thin">
-        <color rgb="FF284E3F"/>
+        <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color rgb="FF284E3F"/>
-      </top>
+      <top/>
       <bottom style="thin">
-        <color rgb="FF284E3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF284E3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF284E3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF284E3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFF6F8F9"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFF6F8F9"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFF6F8F9"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFF6F8F9"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFF6F8F9"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFF6F8F9"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFF6F8F9"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFF6F8F9"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF284E3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFF6F8F9"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFF6F8F9"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF284E3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF284E3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF284E3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF284E3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF284E3F"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -493,51 +395,181 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -566,9 +598,9 @@
   <tableStyles count="1">
     <tableStyle name="Sheet1-style" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" size="0"/>
-      <tableStyleElement type="headerRow" dxfId="2"/>
-      <tableStyleElement type="firstRowStripe" dxfId="1"/>
-      <tableStyleElement type="secondRowStripe" dxfId="0"/>
+      <tableStyleElement type="headerRow" dxfId="9"/>
+      <tableStyleElement type="firstRowStripe" dxfId="8"/>
+      <tableStyleElement type="secondRowStripe" dxfId="7"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -583,14 +615,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F6" dataDxfId="0">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Group Name "/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Volume of Stopper (cm^3)"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Mass of Stopper (g)"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Density (kg m-3)."/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Absolute Uncertainty (kg/m^3)"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Relative Uncertainty (%)"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Group Name " dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Volume of Stopper (cm^3)" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Mass of Stopper (g)" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Density (kg m-3)." dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Absolute Uncertainty (kg/m^3)" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Relative Uncertainty (%)" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="Sheet1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -801,7 +833,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -836,277 +868,277 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="7" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="C3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="D3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="E3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="11">
+      <c r="F3" s="9">
         <v>0.44</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="F4" s="9">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="12">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="E5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="F5" s="9">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E6" s="5"/>
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="11">
-        <v>0.71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="D7" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="E7" s="12">
+        <v>0.7</v>
+      </c>
+      <c r="F7" s="13">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="C8" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="15"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="D8" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="E8" s="12">
+        <v>0.7</v>
+      </c>
+      <c r="F8" s="13">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C9" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D9" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="17">
-        <v>0.7</v>
-      </c>
-      <c r="F7" s="18">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+      <c r="E9" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="F9" s="13">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C10" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D10" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="17">
-        <v>0.7</v>
-      </c>
-      <c r="F8" s="18">
-        <v>0.43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="E10" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="F10" s="13">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="C11" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="D11" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="E11" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="F11" s="13">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="18">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="C12" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="D12" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="E12" s="15">
+        <v>400</v>
+      </c>
+      <c r="F12" s="16">
+        <v>23.57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="C13" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="17">
-        <v>0.2</v>
-      </c>
-      <c r="F10" s="18">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="D13" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="E13" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="F13" s="13">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="C14" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="D14" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="18">
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+      <c r="E14" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="19">
-        <v>400</v>
-      </c>
-      <c r="F12" s="17">
-        <v>23.57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="F13" s="18">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="F14" s="18">
+      <c r="F14" s="13">
         <v>0.23</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="E15" s="17">
+      <c r="B15" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="18">
         <v>0.6</v>
       </c>
-      <c r="F15" s="18">
+      <c r="F15" s="19">
         <v>0.48</v>
       </c>
     </row>
@@ -1119,21 +1151,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001D1BC53C6FCE9A43A8D25BB9995D97C1" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3ba157ab7b56ab4fe2c65fbf4d919c04">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b9e56ef4-41e9-4c5a-acf6-996cf8945303" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3d6bd545251da5e3aa9998f8c8b2b17d" ns2:_="">
     <xsd:import namespace="b9e56ef4-41e9-4c5a-acf6-996cf8945303"/>
@@ -1271,24 +1288,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A35436B-0757-4E81-8D79-C1439EF2B249}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CB13A24-EF9F-40F3-B3DB-D07A5C5E90E8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21DACF78-288C-44E6-B8E8-83CFE67D084E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1304,4 +1319,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CB13A24-EF9F-40F3-B3DB-D07A5C5E90E8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A35436B-0757-4E81-8D79-C1439EF2B249}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>